<commit_message>
Upload README, analyses, and resulting data
</commit_message>
<xml_diff>
--- a/wf_data.xlsx
+++ b/wf_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmgs/Documents/Github/sea-petchem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB043C8-4A88-764E-8432-BC410331B84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3C30E1-796F-C54E-8D79-B95F31B2937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="2060" windowWidth="26620" windowHeight="16260" activeTab="1" xr2:uid="{3B4969AE-2234-774F-A28F-2683FA1E44DB}"/>
+    <workbookView xWindow="1820" yWindow="2060" windowWidth="26620" windowHeight="16260" activeTab="3" xr2:uid="{3B4969AE-2234-774F-A28F-2683FA1E44DB}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="eq_list" sheetId="8" r:id="rId8"/>
     <sheet name="eq_banks" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4730" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="1374">
   <si>
     <t>Announced</t>
   </si>
@@ -3412,9 +3412,6 @@
     <t>book_comanagers_parent</t>
   </si>
   <si>
-    <t>book_comanagers_parent_company</t>
-  </si>
-  <si>
     <t>bonds_banks_id</t>
   </si>
   <si>
@@ -4268,6 +4265,36 @@
   </si>
   <si>
     <t>Upstream / Midstream / Downstream</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>State-owned [PetroChina]</t>
+  </si>
+  <si>
+    <t>State-owned [Petronas]</t>
+  </si>
+  <si>
+    <t>State-owned [DOE]</t>
+  </si>
+  <si>
+    <t>State-owned [Saudi Arabian Oil Co]</t>
+  </si>
+  <si>
+    <t>State-owned [EDB]</t>
+  </si>
+  <si>
+    <t>State-owned [EMA]</t>
+  </si>
+  <si>
+    <t>State-owned [MPA]</t>
+  </si>
+  <si>
+    <t>State-owned [Korea National Oil Corp]</t>
+  </si>
+  <si>
+    <t>State-owned [CPC Corp]</t>
   </si>
 </sst>
 </file>
@@ -4430,7 +4457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4488,6 +4515,9 @@
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4888,15 +4918,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B9" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B10" t="s">
         <v>928</v>
@@ -4904,15 +4934,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B11" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B12" t="s">
         <v>928</v>
@@ -4927,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40768793-6447-D64E-91B8-A1D1ABB0D105}">
   <dimension ref="A1:AB1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V79" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AB6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13240,6 +13270,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -13248,8 +13279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD959BD-EA74-C149-985B-29025CE8DAF4}">
   <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView topLeftCell="B137" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J134" sqref="J134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13819,7 +13850,7 @@
         <v>100</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>362</v>
+        <v>1367</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>21</v>
@@ -13983,7 +14014,7 @@
         <v>33.333300000000001</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>362</v>
+        <v>1369</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>27</v>
@@ -14967,7 +14998,7 @@
         <v>33.333300000000001</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>362</v>
+        <v>1366</v>
       </c>
       <c r="K42" s="16" t="s">
         <v>2</v>
@@ -15090,7 +15121,7 @@
         <v>33.333300000000001</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>362</v>
+        <v>529</v>
       </c>
       <c r="K45" s="16" t="s">
         <v>121</v>
@@ -15582,7 +15613,7 @@
         <v>25</v>
       </c>
       <c r="J57" s="16" t="s">
-        <v>362</v>
+        <v>1365</v>
       </c>
       <c r="K57" s="16" t="s">
         <v>388</v>
@@ -16648,7 +16679,7 @@
         <v>14.2857</v>
       </c>
       <c r="J83" s="16" t="s">
-        <v>362</v>
+        <v>1366</v>
       </c>
       <c r="K83" s="16" t="s">
         <v>2</v>
@@ -16730,7 +16761,7 @@
         <v>50</v>
       </c>
       <c r="J85" s="16" t="s">
-        <v>362</v>
+        <v>1371</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>27</v>
@@ -16771,7 +16802,7 @@
         <v>50</v>
       </c>
       <c r="J86" s="16" t="s">
-        <v>362</v>
+        <v>1370</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>27</v>
@@ -17017,7 +17048,7 @@
         <v>33.332999999999998</v>
       </c>
       <c r="J92" s="16" t="s">
-        <v>362</v>
+        <v>1372</v>
       </c>
       <c r="K92" s="16" t="s">
         <v>350</v>
@@ -17550,7 +17581,7 @@
         <v>20</v>
       </c>
       <c r="J105" s="16" t="s">
-        <v>362</v>
+        <v>1372</v>
       </c>
       <c r="K105" s="16" t="s">
         <v>350</v>
@@ -17868,11 +17899,19 @@
       <c r="F113" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="16"/>
-      <c r="J113" s="16"/>
-      <c r="K113" s="16"/>
+      <c r="G113" s="11" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I113" s="43"/>
+      <c r="J113" s="43" t="s">
+        <v>1364</v>
+      </c>
+      <c r="K113" s="43" t="s">
+        <v>1364</v>
+      </c>
       <c r="L113" s="4" t="s">
         <v>491</v>
       </c>
@@ -17940,11 +17979,19 @@
       <c r="F115" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="16"/>
-      <c r="K115" s="16"/>
+      <c r="G115" s="11" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H115" s="11" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I115" s="43"/>
+      <c r="J115" s="43" t="s">
+        <v>1364</v>
+      </c>
+      <c r="K115" s="43" t="s">
+        <v>1364</v>
+      </c>
       <c r="L115" s="4" t="s">
         <v>494</v>
       </c>
@@ -17981,7 +18028,7 @@
         <v>50</v>
       </c>
       <c r="J116" s="16" t="s">
-        <v>362</v>
+        <v>1373</v>
       </c>
       <c r="K116" s="16" t="s">
         <v>496</v>
@@ -18061,7 +18108,7 @@
       </c>
       <c r="I118" s="18"/>
       <c r="J118" s="18" t="s">
-        <v>362</v>
+        <v>1368</v>
       </c>
       <c r="K118" s="18" t="s">
         <v>373</v>
@@ -18983,8 +19030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C420AB-B889-1545-9030-7F01D544120C}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19064,8 +19111,12 @@
       <c r="F2" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I2" s="29">
         <v>44776</v>
       </c>
@@ -19107,8 +19158,12 @@
       <c r="F3" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I3" s="29">
         <v>44040</v>
       </c>
@@ -19181,7 +19236,7 @@
         <v>832</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -19254,8 +19309,12 @@
       <c r="F6" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I6" s="32">
         <v>43313</v>
       </c>
@@ -19479,8 +19538,12 @@
       <c r="F11" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I11" s="33">
         <v>43313</v>
       </c>
@@ -19520,8 +19583,12 @@
       <c r="F12" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I12" s="33">
         <v>43313</v>
       </c>
@@ -19604,8 +19671,12 @@
       <c r="F14" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="28" t="s">
+        <v>821</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>824</v>
+      </c>
       <c r="I14" s="33">
         <v>43313</v>
       </c>
@@ -20294,8 +20365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1041F363-6D89-7646-ADAD-C488EB250501}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K38" sqref="K22:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22038,8 +22109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D9CF84-92B0-E74B-9E52-5558A17E4247}">
   <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22051,7 +22122,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>964</v>
@@ -22072,12 +22143,12 @@
         <v>1078</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1079</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>965</v>
@@ -22103,7 +22174,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>965</v>
@@ -22129,7 +22200,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>965</v>
@@ -22147,7 +22218,7 @@
         <v>63</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>350</v>
@@ -22155,7 +22226,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>965</v>
@@ -22181,7 +22252,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>966</v>
@@ -22207,7 +22278,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>966</v>
@@ -22233,7 +22304,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>967</v>
@@ -22259,7 +22330,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>967</v>
@@ -22285,7 +22356,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>967</v>
@@ -22311,7 +22382,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>967</v>
@@ -22337,7 +22408,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>967</v>
@@ -22363,7 +22434,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>967</v>
@@ -22389,7 +22460,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>967</v>
@@ -22415,7 +22486,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>967</v>
@@ -22441,7 +22512,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>967</v>
@@ -22467,7 +22538,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>967</v>
@@ -22493,7 +22564,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>967</v>
@@ -22519,7 +22590,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>967</v>
@@ -22545,7 +22616,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>967</v>
@@ -22571,7 +22642,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>967</v>
@@ -22597,7 +22668,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>967</v>
@@ -22623,7 +22694,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>967</v>
@@ -22649,7 +22720,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>967</v>
@@ -22675,7 +22746,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>968</v>
@@ -22701,7 +22772,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>968</v>
@@ -22727,7 +22798,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>968</v>
@@ -22753,7 +22824,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>969</v>
@@ -22779,7 +22850,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>970</v>
@@ -22805,7 +22876,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>970</v>
@@ -22831,7 +22902,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>970</v>
@@ -22857,7 +22928,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>970</v>
@@ -22883,7 +22954,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>970</v>
@@ -22909,7 +22980,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>970</v>
@@ -22935,7 +23006,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>970</v>
@@ -22961,7 +23032,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>970</v>
@@ -22987,7 +23058,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>970</v>
@@ -23013,7 +23084,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>970</v>
@@ -23039,7 +23110,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>970</v>
@@ -23065,7 +23136,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>970</v>
@@ -23091,7 +23162,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>970</v>
@@ -23117,7 +23188,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>970</v>
@@ -23143,7 +23214,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>970</v>
@@ -23169,7 +23240,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>970</v>
@@ -23195,7 +23266,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>970</v>
@@ -23221,7 +23292,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>970</v>
@@ -23247,7 +23318,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>971</v>
@@ -23273,7 +23344,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>971</v>
@@ -23299,7 +23370,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>971</v>
@@ -23325,7 +23396,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>971</v>
@@ -23351,7 +23422,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>972</v>
@@ -23377,7 +23448,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>972</v>
@@ -23403,7 +23474,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>972</v>
@@ -23429,7 +23500,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>972</v>
@@ -23455,7 +23526,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>972</v>
@@ -23481,7 +23552,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>973</v>
@@ -23507,7 +23578,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>973</v>
@@ -23533,7 +23604,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>973</v>
@@ -23559,7 +23630,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>973</v>
@@ -23585,7 +23656,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>973</v>
@@ -23611,7 +23682,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>974</v>
@@ -23637,7 +23708,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>974</v>
@@ -23663,7 +23734,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>974</v>
@@ -23689,7 +23760,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>974</v>
@@ -23715,7 +23786,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>974</v>
@@ -23741,7 +23812,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>974</v>
@@ -23767,7 +23838,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>974</v>
@@ -23793,7 +23864,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>974</v>
@@ -23819,7 +23890,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>974</v>
@@ -23845,7 +23916,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>974</v>
@@ -23871,7 +23942,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>974</v>
@@ -23897,7 +23968,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>974</v>
@@ -23923,7 +23994,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>974</v>
@@ -23949,7 +24020,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>975</v>
@@ -23975,7 +24046,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>975</v>
@@ -24001,7 +24072,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>976</v>
@@ -24027,7 +24098,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>976</v>
@@ -24053,7 +24124,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>976</v>
@@ -24079,7 +24150,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>976</v>
@@ -24105,7 +24176,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>976</v>
@@ -24131,7 +24202,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>976</v>
@@ -24157,7 +24228,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>976</v>
@@ -24183,7 +24254,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>976</v>
@@ -24209,7 +24280,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>977</v>
@@ -24235,7 +24306,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>977</v>
@@ -24261,7 +24332,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>977</v>
@@ -24287,7 +24358,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>977</v>
@@ -24313,7 +24384,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>977</v>
@@ -24339,7 +24410,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>977</v>
@@ -24365,7 +24436,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>977</v>
@@ -24391,7 +24462,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>977</v>
@@ -24417,7 +24488,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>977</v>
@@ -24443,7 +24514,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>977</v>
@@ -24469,7 +24540,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>977</v>
@@ -24495,7 +24566,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>978</v>
@@ -24521,7 +24592,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>978</v>
@@ -24547,7 +24618,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>979</v>
@@ -24573,7 +24644,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>979</v>
@@ -24599,7 +24670,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>980</v>
@@ -24625,7 +24696,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>980</v>
@@ -24651,7 +24722,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>980</v>
@@ -24677,7 +24748,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>980</v>
@@ -24703,7 +24774,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>980</v>
@@ -24729,7 +24800,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>980</v>
@@ -24755,7 +24826,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>980</v>
@@ -24781,7 +24852,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>980</v>
@@ -24807,7 +24878,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>980</v>
@@ -24833,7 +24904,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>980</v>
@@ -24859,7 +24930,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>980</v>
@@ -24885,7 +24956,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>981</v>
@@ -24911,7 +24982,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>981</v>
@@ -24937,7 +25008,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>981</v>
@@ -24963,7 +25034,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>981</v>
@@ -24989,7 +25060,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>981</v>
@@ -25015,7 +25086,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>981</v>
@@ -25041,7 +25112,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>981</v>
@@ -25067,7 +25138,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>981</v>
@@ -25093,7 +25164,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>981</v>
@@ -25119,7 +25190,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>981</v>
@@ -25145,7 +25216,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>982</v>
@@ -25163,7 +25234,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>983</v>
@@ -25189,7 +25260,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>983</v>
@@ -25215,7 +25286,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>983</v>
@@ -25241,7 +25312,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>983</v>
@@ -25267,7 +25338,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B125" s="8" t="s">
         <v>983</v>
@@ -25293,7 +25364,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>983</v>
@@ -25319,7 +25390,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="8" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B127" s="8" t="s">
         <v>983</v>
@@ -25345,7 +25416,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>983</v>
@@ -25371,7 +25442,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>983</v>
@@ -25397,7 +25468,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>984</v>
@@ -25423,7 +25494,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>984</v>
@@ -25449,7 +25520,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>985</v>
@@ -25475,7 +25546,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B133" s="8" t="s">
         <v>985</v>
@@ -25501,7 +25572,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>985</v>
@@ -25527,7 +25598,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>985</v>
@@ -25553,7 +25624,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>985</v>
@@ -25579,7 +25650,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>985</v>
@@ -25605,7 +25676,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>985</v>
@@ -25631,7 +25702,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="8" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>985</v>
@@ -25657,7 +25728,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>985</v>
@@ -25683,7 +25754,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="8" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>986</v>
@@ -25709,7 +25780,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>986</v>
@@ -25735,7 +25806,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="8" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>986</v>
@@ -25761,7 +25832,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>986</v>
@@ -25787,7 +25858,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="8" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>986</v>
@@ -25813,7 +25884,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>986</v>
@@ -25839,7 +25910,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="8" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>987</v>
@@ -25865,7 +25936,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>987</v>
@@ -25891,7 +25962,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="8" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>988</v>
@@ -25917,7 +25988,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="8" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>989</v>
@@ -25943,7 +26014,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>989</v>
@@ -25969,7 +26040,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="8" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>990</v>
@@ -25995,7 +26066,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="8" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>990</v>
@@ -26021,7 +26092,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>991</v>
@@ -26047,7 +26118,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="8" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>991</v>
@@ -26073,7 +26144,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>991</v>
@@ -26099,7 +26170,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="8" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B157" s="8" t="s">
         <v>991</v>
@@ -26125,7 +26196,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="8" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>991</v>
@@ -26151,7 +26222,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B159" s="8" t="s">
         <v>991</v>
@@ -26177,7 +26248,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="8" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>992</v>
@@ -26203,7 +26274,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="8" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>992</v>
@@ -26229,7 +26300,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>992</v>
@@ -26255,7 +26326,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="8" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>992</v>
@@ -26281,7 +26352,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B164" s="8" t="s">
         <v>992</v>
@@ -26307,7 +26378,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>993</v>
@@ -26333,7 +26404,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>993</v>
@@ -26359,7 +26430,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="8" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>993</v>
@@ -26385,7 +26456,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="8" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>994</v>
@@ -26411,7 +26482,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="8" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>994</v>
@@ -26437,7 +26508,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="8" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>994</v>
@@ -26463,7 +26534,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>994</v>
@@ -26489,7 +26560,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>994</v>
@@ -26515,7 +26586,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>995</v>
@@ -26541,7 +26612,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>995</v>
@@ -26567,7 +26638,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="8" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>996</v>
@@ -26593,7 +26664,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>997</v>
@@ -26619,7 +26690,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B177" s="8" t="s">
         <v>998</v>
@@ -26645,7 +26716,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B178" s="8" t="s">
         <v>999</v>
@@ -26671,7 +26742,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="8" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B179" s="8" t="s">
         <v>1000</v>
@@ -26697,7 +26768,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>1000</v>
@@ -26723,7 +26794,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="8" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>1000</v>
@@ -26749,7 +26820,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>1000</v>
@@ -26775,7 +26846,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>1000</v>
@@ -26801,7 +26872,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B184" s="8" t="s">
         <v>1001</v>
@@ -26862,7 +26933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEF8AF7-AC27-494F-8E1D-CC6A399CB6DA}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -26873,10 +26944,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>957</v>
@@ -26900,7 +26971,7 @@
         <v>869</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>960</v>
@@ -26915,7 +26986,7 @@
         <v>963</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>876</v>
@@ -26927,7 +26998,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B2" s="8">
         <v>5540964</v>
@@ -26936,10 +27007,10 @@
         <v>45562</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>1265</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>1266</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>565</v>
@@ -26948,7 +27019,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>2</v>
@@ -26960,16 +27031,16 @@
         <v>2</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>1266</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>1267</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>1268</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>1269</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>1270</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="8" t="s">
@@ -26979,7 +27050,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B3" s="8">
         <v>4990148</v>
@@ -26988,10 +27059,10 @@
         <v>45279</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>931</v>
@@ -27000,7 +27071,7 @@
         <v>101</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>101</v>
@@ -27010,19 +27081,19 @@
         <v>12.8131416837782</v>
       </c>
       <c r="L3" s="8" t="s">
+        <v>1272</v>
+      </c>
+      <c r="M3" s="41" t="s">
         <v>1273</v>
       </c>
-      <c r="M3" s="41" t="s">
-        <v>1274</v>
-      </c>
       <c r="N3" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>1270</v>
-      </c>
       <c r="P3" s="8" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>52</v>
@@ -27031,7 +27102,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B4" s="8">
         <v>5088775</v>
@@ -27040,10 +27111,10 @@
         <v>45224</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>1265</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>1266</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>931</v>
@@ -27052,7 +27123,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>2</v>
@@ -27062,17 +27133,17 @@
         <v>1.9736063635406</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M4" s="41"/>
       <c r="N4" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="O4" s="8" t="s">
-        <v>1270</v>
-      </c>
       <c r="P4" s="8" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="Q4" s="8" t="s">
         <v>131</v>
@@ -27081,7 +27152,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B5" s="8">
         <v>4631663</v>
@@ -27090,19 +27161,19 @@
         <v>44739</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>101</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>101</v>
@@ -27114,16 +27185,16 @@
         <v>21.510002151000201</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M5" s="41" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N5" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>1269</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>1270</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8" t="s">
@@ -27133,7 +27204,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B6" s="8">
         <v>4522267</v>
@@ -27142,10 +27213,10 @@
         <v>44587</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>1277</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>1278</v>
       </c>
       <c r="F6" s="42" t="s">
         <v>306</v>
@@ -27154,7 +27225,7 @@
         <v>121</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>121</v>
@@ -27164,19 +27235,19 @@
       </c>
       <c r="K6" s="41"/>
       <c r="L6" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M6" s="41" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="N6" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>1270</v>
-      </c>
       <c r="P6" s="8" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="Q6" s="42" t="s">
         <v>52</v>
@@ -27185,7 +27256,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B7" s="8">
         <v>4484253</v>
@@ -27194,10 +27265,10 @@
         <v>44571</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>931</v>
@@ -27206,7 +27277,7 @@
         <v>101</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>101</v>
@@ -27218,19 +27289,19 @@
         <v>21.878037453183499</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M7" s="41" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>938</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="Q7" s="42" t="s">
         <v>52</v>
@@ -27239,7 +27310,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B8" s="8">
         <v>4502236</v>
@@ -27248,10 +27319,10 @@
         <v>44557</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>565</v>
@@ -27260,7 +27331,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>2</v>
@@ -27270,17 +27341,17 @@
         <v>11.9588615163836</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M8" s="41"/>
       <c r="N8" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>1269</v>
       </c>
-      <c r="O8" s="8" t="s">
-        <v>1270</v>
-      </c>
       <c r="P8" s="8" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>44</v>
@@ -27289,7 +27360,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B9" s="8">
         <v>4490487</v>
@@ -27301,7 +27372,7 @@
         <v>940</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>0</v>
@@ -27320,14 +27391,14 @@
         <v>1016.2831138914599</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M9" s="41"/>
       <c r="N9" s="8" t="s">
         <v>942</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>943</v>
@@ -27339,7 +27410,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B10" s="8">
         <v>4413593</v>
@@ -27348,10 +27419,10 @@
         <v>44448</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>931</v>
@@ -27372,19 +27443,19 @@
         <v>66.119150988905005</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M10" s="41" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>942</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="Q10" s="8" t="s">
         <v>52</v>
@@ -27393,7 +27464,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B11" s="8">
         <v>3758016</v>
@@ -27405,7 +27476,7 @@
         <v>929</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>931</v>
@@ -27426,16 +27497,16 @@
         <v>96.32</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M11" s="41" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>933</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>934</v>
@@ -27447,7 +27518,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B12" s="8">
         <v>3577109</v>
@@ -27459,7 +27530,7 @@
         <v>929</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>931</v>
@@ -27480,16 +27551,16 @@
         <v>738.10663296999996</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M12" s="41" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>933</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="8" t="s">
@@ -27499,7 +27570,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B13" s="8">
         <v>3565273</v>
@@ -27508,10 +27579,10 @@
         <v>43061</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>565</v>
@@ -27520,7 +27591,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>2</v>
@@ -27532,16 +27603,16 @@
         <v>5.2270437956204399</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M13" s="41" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="N13" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O13" s="8" t="s">
         <v>1269</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>1270</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="8" t="s">
@@ -27551,7 +27622,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B14" s="8">
         <v>3540880</v>
@@ -27560,10 +27631,10 @@
         <v>43049</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>931</v>
@@ -27572,7 +27643,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>2</v>
@@ -27582,14 +27653,14 @@
         <v>2.3673058149669299</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M14" s="41"/>
       <c r="N14" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O14" s="8" t="s">
         <v>1269</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>1270</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8" t="s">
@@ -27599,7 +27670,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B15" s="8">
         <v>3519988</v>
@@ -27608,10 +27679,10 @@
         <v>42996</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>931</v>
@@ -27620,7 +27691,7 @@
         <v>101</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>101</v>
@@ -27632,16 +27703,16 @@
         <v>1.3395237885656399</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M15" s="41" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>938</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="42" t="s">
@@ -27651,7 +27722,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B16" s="8">
         <v>3193945</v>
@@ -27660,10 +27731,10 @@
         <v>42880</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>931</v>
@@ -27672,7 +27743,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>2</v>
@@ -27682,14 +27753,14 @@
         <v>3.9103280866829402</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M16" s="41"/>
       <c r="N16" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="O16" s="8" t="s">
         <v>1269</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>1270</v>
       </c>
       <c r="P16" s="8"/>
       <c r="Q16" s="8" t="s">
@@ -27699,7 +27770,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B17" s="8">
         <v>3282893</v>
@@ -27708,10 +27779,10 @@
         <v>42515</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>931</v>
@@ -27720,7 +27791,7 @@
         <v>21</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>21</v>
@@ -27732,16 +27803,16 @@
         <v>250.95054533789599</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M17" s="8" t="s">
+        <v>1300</v>
+      </c>
+      <c r="N17" s="8" t="s">
         <v>1301</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="O17" s="8" t="s">
         <v>1302</v>
-      </c>
-      <c r="O17" s="8" t="s">
-        <v>1303</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8" t="s">
@@ -27751,7 +27822,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B18" s="8">
         <v>3265927</v>
@@ -27760,19 +27831,19 @@
         <v>42483</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>101</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>101</v>
@@ -27784,16 +27855,16 @@
         <v>8.9823048594269306</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>938</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="8" t="s">
@@ -27884,7 +27955,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27894,13 +27965,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>864</v>
@@ -27915,24 +27986,24 @@
         <v>1078</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C2" s="8">
         <v>5540964</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>2</v>
@@ -27946,19 +28017,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C3" s="8">
         <v>4990148</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -27966,19 +28037,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C4" s="8">
         <v>5088775</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>2</v>
@@ -27992,19 +28063,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C5" s="8">
         <v>4631663</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -28012,19 +28083,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C6" s="8">
         <v>4522267</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -28032,19 +28103,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C7" s="8">
         <v>4484253</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -28052,25 +28123,25 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C8" s="8">
         <v>4502236</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>1282</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>1283</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>2</v>
@@ -28078,10 +28149,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C9" s="8">
         <v>4490487</v>
@@ -28090,7 +28161,7 @@
         <v>940</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -28098,25 +28169,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C10" s="8">
         <v>4413593</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>2</v>
@@ -28124,10 +28195,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C11" s="8">
         <v>3758016</v>
@@ -28136,7 +28207,7 @@
         <v>929</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -28144,10 +28215,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C12" s="8">
         <v>3577109</v>
@@ -28156,13 +28227,13 @@
         <v>929</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>63</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>383</v>
@@ -28170,10 +28241,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C13" s="8">
         <v>3577109</v>
@@ -28182,13 +28253,13 @@
         <v>929</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>63</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>356</v>
@@ -28196,10 +28267,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C14" s="8">
         <v>3577109</v>
@@ -28208,13 +28279,13 @@
         <v>929</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>63</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>341</v>
@@ -28222,25 +28293,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C15" s="8">
         <v>3565273</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>1282</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>1283</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>2</v>
@@ -28248,25 +28319,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C16" s="8">
         <v>3540880</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>1282</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>1283</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>2</v>
@@ -28274,19 +28345,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C17" s="8">
         <v>3519988</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -28294,25 +28365,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C18" s="8">
         <v>3193945</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>1282</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>1283</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>2</v>
@@ -28320,45 +28391,45 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C19" s="8">
         <v>3282893</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>1355</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="C20" s="8">
         <v>3265927</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>

</xml_diff>